<commit_message>
Edit and format the excel table of cyber resources
</commit_message>
<xml_diff>
--- a/quickstart/_drafts/cyberresources_table.xlsx
+++ b/quickstart/_drafts/cyberresources_table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>CYBER RESOURCES TABLE</t>
   </si>
@@ -44,18 +44,9 @@
     <t>Storing code and packages</t>
   </si>
   <si>
-    <t>Try to keep it under 25 GB</t>
-  </si>
-  <si>
     <t>/research-home/&lt;your user name&gt;</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>It's the default working directory when you log into the Rstudio server, Jupyter server, or SSH gateway</t>
-  </si>
-  <si>
     <t>Who has one?</t>
   </si>
   <si>
@@ -68,27 +59,9 @@
     <t>Storing data</t>
   </si>
   <si>
-    <t>Try to keep it under 2 or 3 TB</t>
-  </si>
-  <si>
-    <t>All SESYNC groups; postdocs and staff also have their own</t>
-  </si>
-  <si>
     <t>/nfs/&lt;group name&gt;-data</t>
   </si>
   <si>
-    <t>Connect to it under the "Files" tab in Rstudio server, access via files.sesync.org, or use the SSH gateway ** add how to access it via Jupyter</t>
-  </si>
-  <si>
-    <t>DATA STORAGE</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS</t>
-  </si>
-  <si>
-    <t>Rstudio server</t>
-  </si>
-  <si>
     <t>Jupyter server</t>
   </si>
   <si>
@@ -98,50 +71,164 @@
     <t>Databases</t>
   </si>
   <si>
-    <t>Cyberhelp will create databases for a user or group upon request</t>
-  </si>
-  <si>
     <t>Storing data and establishing formal relationships between datasets</t>
   </si>
   <si>
-    <t>Running code interactively in R</t>
-  </si>
-  <si>
-    <t>Running code interactively in Python</t>
-  </si>
-  <si>
     <t>Running time-intensive or memory-intensive computing jobs in parallel, using any program</t>
   </si>
   <si>
-    <t>How much capacity?</t>
-  </si>
-  <si>
     <t>rstudio.sesync.org</t>
   </si>
   <si>
     <t>jupyter.sesync.org</t>
   </si>
   <si>
-    <t>Through the Rstudio interface in your browser</t>
-  </si>
-  <si>
-    <t>Through the Jupyter interface in your browser</t>
-  </si>
-  <si>
-    <t>Either through the command line via SSH, or through Rstudio with the rslurm package</t>
-  </si>
-  <si>
-    <t>24 cores with 64 to 128 GB memory each</t>
-  </si>
-  <si>
-    <t>xx cores with xx GB memory total</t>
+    <t>(accessed from other SESYNC servers)</t>
+  </si>
+  <si>
+    <t>varies</t>
+  </si>
+  <si>
+    <t>All SESYNC groups and postdocs</t>
+  </si>
+  <si>
+    <t>Created upon request</t>
+  </si>
+  <si>
+    <t>Virtual machines</t>
+  </si>
+  <si>
+    <t>Running commercial or Windows-only software programs</t>
+  </si>
+  <si>
+    <t>desktop.sesync.org</t>
+  </si>
+  <si>
+    <t>Through your browser</t>
+  </si>
+  <si>
+    <t>Try to keep it under ~25 GB</t>
+  </si>
+  <si>
+    <t>Try to keep it under ~3 TB</t>
+  </si>
+  <si>
+    <t>&lt;hostname&gt;.research.sesync.org</t>
+  </si>
+  <si>
+    <t>It's the default working directory when you log into the RStudio server, Jupyter server, or SSH gateway</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Connect to it under the "Files" tab in RStudio server, access via </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>files.sesync.org</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t>, use the SSH gateway, or use a symlink on the Jupyter server</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Connect through RStudio (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>RPostgres</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> package), Python (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>psycopg2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> package), or SSH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Through the command line via SSH, or through RStudio with the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>rslurm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> package</t>
+    </r>
+  </si>
+  <si>
+    <t>Where is it?</t>
+  </si>
+  <si>
+    <t>Table 1: Storing and accessing data</t>
+  </si>
+  <si>
+    <t>Table 2: Running code and analyzing data</t>
+  </si>
+  <si>
+    <t>RStudio server</t>
+  </si>
+  <si>
+    <t>Running Python code interactively</t>
+  </si>
+  <si>
+    <t>Running R code interactively</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,23 +237,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bitter"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bitter"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Tw Cen MT"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -174,17 +291,150 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,168 +716,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="37.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="36.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="D17" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="18" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>34</v>
+      <c r="E18" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweak text and formatting of excel table
</commit_message>
<xml_diff>
--- a/quickstart/_drafts/cyberresources_table.xlsx
+++ b/quickstart/_drafts/cyberresources_table.xlsx
@@ -41,12 +41,6 @@
     <t>Home directory</t>
   </si>
   <si>
-    <t>Storing code and packages</t>
-  </si>
-  <si>
-    <t>/research-home/&lt;your user name&gt;</t>
-  </si>
-  <si>
     <t>Who has one?</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t>Storing data</t>
   </si>
   <si>
-    <t>/nfs/&lt;group name&gt;-data</t>
-  </si>
-  <si>
     <t>Jupyter server</t>
   </si>
   <si>
@@ -71,12 +62,6 @@
     <t>Databases</t>
   </si>
   <si>
-    <t>Storing data and establishing formal relationships between datasets</t>
-  </si>
-  <si>
-    <t>Running time-intensive or memory-intensive computing jobs in parallel, using any program</t>
-  </si>
-  <si>
     <t>rstudio.sesync.org</t>
   </si>
   <si>
@@ -86,9 +71,6 @@
     <t>(accessed from other SESYNC servers)</t>
   </si>
   <si>
-    <t>varies</t>
-  </si>
-  <si>
     <t>All SESYNC groups and postdocs</t>
   </si>
   <si>
@@ -104,18 +86,6 @@
     <t>desktop.sesync.org</t>
   </si>
   <si>
-    <t>Through your browser</t>
-  </si>
-  <si>
-    <t>Try to keep it under ~25 GB</t>
-  </si>
-  <si>
-    <t>Try to keep it under ~3 TB</t>
-  </si>
-  <si>
-    <t>&lt;hostname&gt;.research.sesync.org</t>
-  </si>
-  <si>
     <t>It's the default working directory when you log into the RStudio server, Jupyter server, or SSH gateway</t>
   </si>
   <si>
@@ -221,14 +191,119 @@
     <t>Running Python code interactively</t>
   </si>
   <si>
-    <t>Running R code interactively</t>
+    <t>Try to keep it under ~2 TB</t>
+  </si>
+  <si>
+    <t>Try to keep it under ~10 GB</t>
+  </si>
+  <si>
+    <t>Through your web browser</t>
+  </si>
+  <si>
+    <t>Running R code interactively; submitting Slurm jobs</t>
+  </si>
+  <si>
+    <t>Storing code</t>
+  </si>
+  <si>
+    <t>Running time-intensive or memory-intensive computing jobs in parallel</t>
+  </si>
+  <si>
+    <t>Storing data in a formal relational structure</t>
+  </si>
+  <si>
+    <t>Varies</t>
+  </si>
+  <si>
+    <r>
+      <t>/research-home/&lt;your user name&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t>example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> /research-home/eostrom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/nfs/&lt;group name&gt;-data 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t>example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> /nfs/cooltrees-data/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;hostname&gt;.research.sesync.org 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Bitter"/>
+        <family val="3"/>
+      </rPr>
+      <t>example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> cooltrees.research.sesync.org</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +336,13 @@
       <color theme="1"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bitter"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -716,209 +798,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="B1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="36.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+      <c r="C5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="E7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="B15" s="9"/>
       <c r="C15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D17" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E17" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>26</v>
+      <c r="F18" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create html version of formated cyber table this was done by exporting excel table as web page then manually editing html
</commit_message>
<xml_diff>
--- a/quickstart/_drafts/cyberresources_table.xlsx
+++ b/quickstart/_drafts/cyberresources_table.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="storing and accessing data" sheetId="1" r:id="rId1"/>
+    <sheet name="running code and analyzing data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
-  <si>
-    <t>CYBER RESOURCES TABLE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>What is it for?</t>
   </si>
@@ -177,12 +175,6 @@
   </si>
   <si>
     <t>Where is it?</t>
-  </si>
-  <si>
-    <t>Table 1: Storing and accessing data</t>
-  </si>
-  <si>
-    <t>Table 2: Running code and analyzing data</t>
   </si>
   <si>
     <t>RStudio server</t>
@@ -798,216 +790,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F18"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="23.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" style="3" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
+    <row r="3" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-      <c r="C5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>11</v>
-      </c>
+    <row r="4" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
-    <row r="6" spans="2:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
+    <row r="5" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="D5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
-    <row r="7" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4"/>
+    <row r="6" spans="1:5" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
-    <row r="8" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="2:6" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B15" s="9"/>
-      <c r="C15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>31</v>
-      </c>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <webPublishItems count="1">
+    <webPublishItem id="1490" divId="cyberresources_table_1490" sourceType="sheet" destinationFile="C:\Users\qread\Documents\GitHub\sesync_repos\sesync-ci.github.io\quickstart\_drafts\cyberresources_table1.htm" title="Storing and accessing data"/>
+  </webPublishItems>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <webPublishItems count="1">
+    <webPublishItem id="9331" divId="cyberresources_table_9331" sourceType="sheet" destinationFile="C:\Users\qread\Documents\GitHub\sesync_repos\sesync-ci.github.io\quickstart\_drafts\cyberresources_table2.htm" title="Running code and analyzing data"/>
+  </webPublishItems>
 </worksheet>
 </file>
</xml_diff>